<commit_message>
update configuration and menu files
</commit_message>
<xml_diff>
--- a/Marlin/Menu Plans.xlsx
+++ b/Marlin/Menu Plans.xlsx
@@ -1,21 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7665" yWindow="-15" windowWidth="7710" windowHeight="8235" activeTab="1"/>
+    <workbookView xWindow="7660" yWindow="-20" windowWidth="8000" windowHeight="8240" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Menus V1" sheetId="3" r:id="rId1"/>
     <sheet name="Menu Tree" sheetId="4" r:id="rId2"/>
+    <sheet name="Menus V1 CN" sheetId="5" r:id="rId3"/>
+    <sheet name="Menu Tree CN" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="105">
   <si>
     <t>Main Screen</t>
   </si>
@@ -177,13 +184,217 @@
   </si>
   <si>
     <t>Marlin LCD Menu Tree (V1)</t>
+  </si>
+  <si>
+    <t>信息界面</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Marlin LCD Menu Tree 中文版 (V1)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>准备</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>控制</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>存储卡菜单</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>主菜单</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>主菜单</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>自动开始</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>关闭步进驱动</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>自动回原点</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>设定原点</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>预热 PLA</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>预热 ABS</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>降温</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动轴</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>温度</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>运动</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>PLA预热设定</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ABS预热设定</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>运动</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存参数</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>载入参数</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>恢复出厂设定</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>刷新</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>挤出</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>回收</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>挤出头</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>自动控温</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>因数</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>热床</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>风扇速度</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>加速度:</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小移动速度</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小速度</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大速度X</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大速度Y</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大速度Z</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大速度E</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大加速度X</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大加速度E</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大加速度Z</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大加速度Y</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>E回收加速度</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>X轴步每mm</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>E轴步每mm</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Z轴步每mm</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y轴步每mm</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>加热头</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存参数</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -218,6 +429,30 @@
       <name val="LCD Display Grid"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <name val="LCD Display Grid"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -248,10 +483,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -265,9 +510,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="11">
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -371,7 +631,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="'Menus V1'!$A$1:$A$7" spid="_x0000_s4257"/>
+                  <a14:cameraTool cellRange="'Menus V1'!$A$1:$A$7" spid="_x0000_s4365"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -402,7 +662,7 @@
               </a:outerShdw>
             </a:effectLst>
             <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
                     <a:srgbClr val="FFFFFF"/>
@@ -555,7 +815,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="'Menus V1'!$C$1:$C$9" spid="_x0000_s4258"/>
+                  <a14:cameraTool cellRange="'Menus V1'!$C$1:$C$9" spid="_x0000_s4366"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -586,7 +846,7 @@
               </a:outerShdw>
             </a:effectLst>
             <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
                     <a:srgbClr val="FFFFFF"/>
@@ -623,7 +883,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="'Menus V1'!$D$1:$D$5" spid="_x0000_s4259"/>
+                  <a14:cameraTool cellRange="'Menus V1'!$D$1:$D$5" spid="_x0000_s4367"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -654,7 +914,7 @@
               </a:outerShdw>
             </a:effectLst>
             <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
                     <a:srgbClr val="FFFFFF"/>
@@ -865,8 +1125,8 @@
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="7063212" y="848590"/>
-              <a:ext cx="1945748" cy="7829041"/>
+              <a:off x="7946439" y="762000"/>
+              <a:ext cx="2142021" cy="8123449"/>
               <a:chOff x="7314378" y="813954"/>
               <a:chExt cx="1945748" cy="7829041"/>
             </a:xfrm>
@@ -878,7 +1138,7 @@
                 <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
                 <a:extLst>
                   <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                    <a14:cameraTool cellRange="'Menus V1'!$E$1:$E$9" spid="_x0000_s4260"/>
+                    <a14:cameraTool cellRange="'Menus V1'!$E$1:$E$9" spid="_x0000_s4368"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPicPr>
@@ -909,7 +1169,7 @@
                 </a:outerShdw>
               </a:effectLst>
               <a:extLst>
-                <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
                   <a14:hiddenFill>
                     <a:solidFill>
                       <a:srgbClr val="FFFFFF"/>
@@ -926,7 +1186,7 @@
                 <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
                 <a:extLst>
                   <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                    <a14:cameraTool cellRange="'Menus V1'!$F$1:$F$17" spid="_x0000_s4261"/>
+                    <a14:cameraTool cellRange="'Menus V1'!$F$1:$F$17" spid="_x0000_s4369"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPicPr>
@@ -957,7 +1217,7 @@
                 </a:outerShdw>
               </a:effectLst>
               <a:extLst>
-                <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
                   <a14:hiddenFill>
                     <a:solidFill>
                       <a:srgbClr val="FFFFFF"/>
@@ -974,7 +1234,7 @@
                 <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
                 <a:extLst>
                   <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                    <a14:cameraTool cellRange="'Menus V1'!$G$1:$G$20" spid="_x0000_s4262"/>
+                    <a14:cameraTool cellRange="'Menus V1'!$G$1:$G$20" spid="_x0000_s4370"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPicPr>
@@ -1005,7 +1265,7 @@
                 </a:outerShdw>
               </a:effectLst>
               <a:extLst>
-                <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
                   <a14:hiddenFill>
                     <a:solidFill>
                       <a:srgbClr val="FFFFFF"/>
@@ -1217,8 +1477,8 @@
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="10607861" y="2272903"/>
-              <a:ext cx="1939636" cy="2719099"/>
+              <a:off x="11883634" y="2244039"/>
+              <a:ext cx="2234045" cy="2817235"/>
               <a:chOff x="10607861" y="2238266"/>
               <a:chExt cx="1939636" cy="2719099"/>
             </a:xfrm>
@@ -1230,7 +1490,7 @@
                 <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
                 <a:extLst>
                   <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                    <a14:cameraTool cellRange="'Menus V1'!$I$1:$I$8" spid="_x0000_s4263"/>
+                    <a14:cameraTool cellRange="'Menus V1'!$I$1:$I$8" spid="_x0000_s4371"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPicPr>
@@ -1261,7 +1521,7 @@
                 </a:outerShdw>
               </a:effectLst>
               <a:extLst>
-                <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
                   <a14:hiddenFill>
                     <a:solidFill>
                       <a:srgbClr val="FFFFFF"/>
@@ -1278,7 +1538,7 @@
                 <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
                 <a:extLst>
                   <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                    <a14:cameraTool cellRange="'Menus V1'!$H$1:$H$8" spid="_x0000_s4264"/>
+                    <a14:cameraTool cellRange="'Menus V1'!$H$1:$H$8" spid="_x0000_s4372"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPicPr>
@@ -1309,7 +1569,7 @@
                 </a:outerShdw>
               </a:effectLst>
               <a:extLst>
-                <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
                   <a14:hiddenFill>
                     <a:solidFill>
                       <a:srgbClr val="FFFFFF"/>
@@ -1368,7 +1628,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1380,6 +1640,1087 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>800100</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>52229</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>280190</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>69091</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Picture 1"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="'Menus V1 CN'!$A$1:$A$7" spid="_x0000_s7258"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="2552700" y="674529"/>
+              <a:ext cx="2108990" cy="1083662"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="292100" dist="139700" dir="2700000" algn="tl" rotWithShape="0">
+                <a:srgbClr val="333333">
+                  <a:alpha val="65000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>242638</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>69091</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>101995</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142324</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 5"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="2"/>
+          <a:endCxn id="24" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="1">
+          <a:off x="1118938" y="1758191"/>
+          <a:ext cx="2488257" cy="682833"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln cap="rnd">
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="292100" dist="139700" dir="2700000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="65000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4291</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>69091</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>101995</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>15324</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 15"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="2"/>
+          <a:endCxn id="5" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="1">
+          <a:off x="3509491" y="1758191"/>
+          <a:ext cx="97704" cy="708233"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln cap="rnd">
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="292100" dist="139700" dir="2700000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="65000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>637953</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>15324</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>246928</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>139699</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="5" name="Picture 14"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="'Menus V1 CN'!$C$1:$C$9" spid="_x0000_s7259"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="2390553" y="2466424"/>
+              <a:ext cx="2237875" cy="1495975"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="292100" dist="139700" dir="2700000" algn="tl" rotWithShape="0">
+                <a:srgbClr val="333333">
+                  <a:alpha val="65000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>383952</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>17663</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>751476</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>120649</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="6" name="Picture 23"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="'Menus V1 CN'!$D$1:$D$5" spid="_x0000_s7260"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="4765452" y="2468763"/>
+              <a:ext cx="2120124" cy="712586"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="292100" dist="139700" dir="2700000" algn="tl" rotWithShape="0">
+                <a:srgbClr val="333333">
+                  <a:alpha val="65000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>101995</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>69091</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>567714</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>17663</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 24"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="2"/>
+          <a:endCxn id="6" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3607195" y="1758191"/>
+          <a:ext cx="2218319" cy="710572"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln cap="rnd">
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="292100" dist="139700" dir="2700000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="65000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>242638</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>127001</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>243036</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>100445</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 28"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="24" idx="2"/>
+          <a:endCxn id="11" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1118938" y="4254501"/>
+          <a:ext cx="398" cy="430644"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln cap="rnd">
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="292100" dist="139700" dir="2700000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="65000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>788410</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>139699</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4291</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>53810</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 32"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="2"/>
+          <a:endCxn id="12" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="1">
+          <a:off x="3417310" y="3962399"/>
+          <a:ext cx="92181" cy="371311"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln cap="rnd">
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="292100" dist="139700" dir="2700000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="65000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>50800</xdr:colOff>
+          <xdr:row>28</xdr:row>
+          <xdr:rowOff>100445</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>435272</xdr:colOff>
+          <xdr:row>37</xdr:row>
+          <xdr:rowOff>109276</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="11" name="Picture 27"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="'Menus V1 CN'!$E$1:$E$9" spid="_x0000_s7261"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="50800" y="4685145"/>
+              <a:ext cx="2137072" cy="1380431"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="292100" dist="139700" dir="2700000" algn="tl" rotWithShape="0">
+                <a:srgbClr val="333333">
+                  <a:alpha val="65000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>558800</xdr:colOff>
+          <xdr:row>26</xdr:row>
+          <xdr:rowOff>53810</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>141720</xdr:colOff>
+          <xdr:row>43</xdr:row>
+          <xdr:rowOff>129445</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="12" name="Picture 31"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="'Menus V1 CN'!$F$1:$F$17" spid="_x0000_s7262"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="2311400" y="4333710"/>
+              <a:ext cx="2211820" cy="2666435"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="292100" dist="139700" dir="2700000" algn="tl" rotWithShape="0">
+                <a:srgbClr val="333333">
+                  <a:alpha val="65000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>354148</xdr:colOff>
+          <xdr:row>26</xdr:row>
+          <xdr:rowOff>73978</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>741260</xdr:colOff>
+          <xdr:row>47</xdr:row>
+          <xdr:rowOff>31240</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="13" name="Picture 38"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="'Menus V1 CN'!$G$1:$G$20" spid="_x0000_s7263"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="4735648" y="4353878"/>
+              <a:ext cx="2139712" cy="3157662"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="292100" dist="139700" dir="2700000" algn="tl" rotWithShape="0">
+                <a:srgbClr val="333333">
+                  <a:alpha val="65000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4291</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>139699</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>547704</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>73978</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 39"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="2"/>
+          <a:endCxn id="13" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3509491" y="3962399"/>
+          <a:ext cx="2296013" cy="391479"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln cap="rnd">
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="292100" dist="139700" dir="2700000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="65000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>461716</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>129445</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>788410</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>143921</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 45"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="12" idx="2"/>
+          <a:endCxn id="19" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="1">
+          <a:off x="2214316" y="7000145"/>
+          <a:ext cx="1202994" cy="624076"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln cap="rnd">
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="292100" dist="139700" dir="2700000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="65000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>788410</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>129445</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>156916</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>136432</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 46"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="12" idx="2"/>
+          <a:endCxn id="18" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3417310" y="7000145"/>
+          <a:ext cx="1121106" cy="616587"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln cap="rnd">
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="292100" dist="139700" dir="2700000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="65000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>794225</xdr:colOff>
+          <xdr:row>47</xdr:row>
+          <xdr:rowOff>136432</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>395906</xdr:colOff>
+          <xdr:row>55</xdr:row>
+          <xdr:rowOff>137138</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="18" name="Picture 49"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="'Menus V1 CN'!$I$1:$I$8" spid="_x0000_s7264"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="3423125" y="7616732"/>
+              <a:ext cx="2230581" cy="1219906"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="292100" dist="139700" dir="2700000" algn="tl" rotWithShape="0">
+                <a:srgbClr val="333333">
+                  <a:alpha val="65000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>222725</xdr:colOff>
+          <xdr:row>47</xdr:row>
+          <xdr:rowOff>143921</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>700706</xdr:colOff>
+          <xdr:row>55</xdr:row>
+          <xdr:rowOff>144630</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="19" name="Picture 54"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="'Menus V1 CN'!$H$1:$H$8" spid="_x0000_s7265"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="1099025" y="7624221"/>
+              <a:ext cx="2230581" cy="1219909"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="292100" dist="139700" dir="2700000" algn="tl" rotWithShape="0">
+                <a:srgbClr val="333333">
+                  <a:alpha val="65000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>142324</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>485275</xdr:colOff>
+          <xdr:row>25</xdr:row>
+          <xdr:rowOff>127001</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="24" name="Picture 14"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="'Menus V1 CN'!$B$1:$B$11" spid="_x0000_s7266"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="2441024"/>
+              <a:ext cx="2237875" cy="1813477"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="292100" dist="139700" dir="2700000" algn="tl" rotWithShape="0">
+                <a:srgbClr val="333333">
+                  <a:alpha val="65000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -1692,7 +3033,7 @@
         </a:ln>
         <a:effectLst/>
         <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+          <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
             <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
@@ -1734,7 +3075,7 @@
         </a:ln>
         <a:effectLst/>
         <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+          <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
             <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
@@ -1757,14 +3098,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B12"/>
+    <sheetView topLeftCell="E1" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="9" width="28.7109375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5703125" style="1"/>
+    <col min="1" max="9" width="28.6640625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1">
@@ -2145,12 +3486,18 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2158,13 +3505,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="H45" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="44.25">
+    <row r="1" spans="1:16" ht="37">
       <c r="A1" s="6" t="s">
         <v>53</v>
       </c>
@@ -2189,11 +3536,469 @@
   <mergeCells count="1">
     <mergeCell ref="A1:P1"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" fitToWidth="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="8" fitToWidth="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="9" width="28.6640625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.5" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="5" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="6.75" customHeight="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:P1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A29" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:16" ht="37">
+      <c r="A1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="78" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>